<commit_message>
Added Stricter Marketing policies for Model 4
</commit_message>
<xml_diff>
--- a/model_data.xlsx
+++ b/model_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ja\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76A2477-2C53-47DF-A4E9-F6DDB11B5E84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB553EC5-9469-476A-8DC4-4A2887E5881A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6230" xr2:uid="{261FA09F-BE23-4540-BC1B-5BD0B21A542F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="35">
   <si>
     <t>Estonia</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>Lower taxation and/or increased availability</t>
+  </si>
+  <si>
+    <t>Stricter marketing policy</t>
+  </si>
+  <si>
+    <t>Restrictions on alcohol marketing</t>
   </si>
 </sst>
 </file>
@@ -251,8 +257,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DA60A27-CCF1-43BA-9993-9CA7F3756CF8}" name="Tabela1" displayName="Tabela1" ref="A1:B9" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A1:B9" xr:uid="{5371A010-12D3-4C2B-8911-7F4F7F734E3D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4DA60A27-CCF1-43BA-9993-9CA7F3756CF8}" name="Tabela1" displayName="Tabela1" ref="A1:B10" totalsRowShown="0" dataDxfId="2">
+  <autoFilter ref="A1:B10" xr:uid="{5371A010-12D3-4C2B-8911-7F4F7F734E3D}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D212321F-00B3-4603-90DD-25D9ADF1273F}" name="Nazwa zmiennej" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{9B3131C8-F658-44DA-B06F-4F8E99721AE5}" name="objaśnienie" dataDxfId="0"/>
@@ -558,19 +564,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695E14F5-B72F-4225-A515-E8F798D9F817}">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="7" max="7" width="18.6328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -595,8 +600,11 @@
       <c r="H1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10.19</v>
       </c>
@@ -621,8 +629,11 @@
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11.77</v>
       </c>
@@ -647,8 +658,11 @@
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>11.35</v>
       </c>
@@ -673,8 +687,11 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>14.36</v>
       </c>
@@ -699,8 +716,11 @@
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>15.18</v>
       </c>
@@ -725,8 +745,11 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>16.190000000000001</v>
       </c>
@@ -751,8 +774,11 @@
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>15.85</v>
       </c>
@@ -777,8 +803,11 @@
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>15.47</v>
       </c>
@@ -803,8 +832,11 @@
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>13.93</v>
       </c>
@@ -829,8 +861,11 @@
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>13.87</v>
       </c>
@@ -855,8 +890,11 @@
       <c r="H11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>14.88</v>
       </c>
@@ -881,8 +919,11 @@
       <c r="H12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>15.42</v>
       </c>
@@ -907,8 +948,11 @@
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>16.05</v>
       </c>
@@ -933,8 +977,11 @@
       <c r="H14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>15.67</v>
       </c>
@@ -959,8 +1006,11 @@
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15.21</v>
       </c>
@@ -985,8 +1035,11 @@
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>14.3</v>
       </c>
@@ -1011,8 +1064,11 @@
       <c r="H17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>12.27</v>
       </c>
@@ -1037,8 +1093,11 @@
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>10.44</v>
       </c>
@@ -1063,8 +1122,11 @@
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>11.09</v>
       </c>
@@ -1089,8 +1151,11 @@
       <c r="H20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>11.17</v>
       </c>
@@ -1115,8 +1180,11 @@
       <c r="H21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>8.5399999999999991</v>
       </c>
@@ -1141,8 +1209,11 @@
       <c r="H22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>9.16</v>
       </c>
@@ -1167,8 +1238,11 @@
       <c r="H23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>9.7899999999999991</v>
       </c>
@@ -1193,8 +1267,11 @@
       <c r="H24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>10.220000000000001</v>
       </c>
@@ -1219,8 +1296,11 @@
       <c r="H25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>11.05</v>
       </c>
@@ -1245,8 +1325,11 @@
       <c r="H26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>11.39</v>
       </c>
@@ -1271,8 +1354,11 @@
       <c r="H27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>12.68</v>
       </c>
@@ -1297,8 +1383,11 @@
       <c r="H28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>12.44</v>
       </c>
@@ -1323,8 +1412,11 @@
       <c r="H29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>10.94</v>
       </c>
@@ -1349,8 +1441,11 @@
       <c r="H30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>10.91</v>
       </c>
@@ -1375,8 +1470,11 @@
       <c r="H31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>11.1</v>
       </c>
@@ -1401,8 +1499,11 @@
       <c r="H32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>11.13</v>
       </c>
@@ -1427,8 +1528,11 @@
       <c r="H33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>11.28</v>
       </c>
@@ -1453,8 +1557,11 @@
       <c r="H34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>11.39</v>
       </c>
@@ -1479,8 +1586,11 @@
       <c r="H35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>11.53</v>
       </c>
@@ -1505,8 +1615,11 @@
       <c r="H36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>11.89</v>
       </c>
@@ -1531,8 +1644,11 @@
       <c r="H37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>12.88</v>
       </c>
@@ -1557,8 +1673,11 @@
       <c r="H38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>13.32</v>
       </c>
@@ -1583,8 +1702,11 @@
       <c r="H39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>13.07</v>
       </c>
@@ -1609,8 +1731,11 @@
       <c r="H40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>12.92</v>
       </c>
@@ -1635,8 +1760,11 @@
       <c r="H41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>11.34</v>
       </c>
@@ -1661,8 +1789,11 @@
       <c r="H42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>12.07</v>
       </c>
@@ -1687,8 +1818,11 @@
       <c r="H43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>12.32</v>
       </c>
@@ -1713,8 +1847,11 @@
       <c r="H44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>13.05</v>
       </c>
@@ -1739,8 +1876,11 @@
       <c r="H45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>13.34</v>
       </c>
@@ -1765,8 +1905,11 @@
       <c r="H46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>14.16</v>
       </c>
@@ -1791,8 +1934,11 @@
       <c r="H47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>14.55</v>
       </c>
@@ -1817,8 +1963,11 @@
       <c r="H48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>14.53</v>
       </c>
@@ -1843,8 +1992,11 @@
       <c r="H49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>13.8</v>
       </c>
@@ -1869,8 +2021,11 @@
       <c r="H50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>12.91</v>
       </c>
@@ -1895,8 +2050,11 @@
       <c r="H51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>15.44</v>
       </c>
@@ -1921,8 +2079,11 @@
       <c r="H52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>15.62</v>
       </c>
@@ -1947,8 +2108,11 @@
       <c r="H53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>15.56</v>
       </c>
@@ -1973,8 +2137,11 @@
       <c r="H54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>15.53</v>
       </c>
@@ -1999,8 +2166,11 @@
       <c r="H55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>13.79</v>
       </c>
@@ -2025,8 +2195,11 @@
       <c r="H56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>13.19</v>
       </c>
@@ -2051,8 +2224,11 @@
       <c r="H57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>12.09</v>
       </c>
@@ -2077,8 +2253,11 @@
       <c r="H58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>11.57</v>
       </c>
@@ -2103,8 +2282,11 @@
       <c r="H59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>11.69</v>
       </c>
@@ -2129,8 +2311,11 @@
       <c r="H60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>12.1</v>
       </c>
@@ -2155,8 +2340,11 @@
       <c r="H61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>9.36</v>
       </c>
@@ -2181,8 +2369,11 @@
       <c r="H62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>9.6</v>
       </c>
@@ -2207,8 +2398,11 @@
       <c r="H63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>10.5</v>
       </c>
@@ -2233,8 +2427,11 @@
       <c r="H64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>10.6</v>
       </c>
@@ -2259,8 +2456,11 @@
       <c r="H65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>10.48</v>
       </c>
@@ -2285,8 +2485,11 @@
       <c r="H66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>11.03</v>
       </c>
@@ -2311,8 +2514,11 @@
       <c r="H67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>11.56</v>
       </c>
@@ -2337,8 +2543,11 @@
       <c r="H68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>11.89</v>
       </c>
@@ -2363,8 +2572,11 @@
       <c r="H69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>11.33</v>
       </c>
@@ -2389,8 +2601,11 @@
       <c r="H70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>11.22</v>
       </c>
@@ -2415,8 +2630,11 @@
       <c r="H71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>11.34</v>
       </c>
@@ -2441,8 +2659,11 @@
       <c r="H72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>11.3</v>
       </c>
@@ -2467,8 +2688,11 @@
       <c r="H73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>11.79</v>
       </c>
@@ -2493,8 +2717,11 @@
       <c r="H74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>11.48</v>
       </c>
@@ -2519,8 +2746,11 @@
       <c r="H75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>11.48</v>
       </c>
@@ -2545,8 +2775,11 @@
       <c r="H76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>11.42</v>
       </c>
@@ -2571,8 +2804,11 @@
       <c r="H77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>11.5</v>
       </c>
@@ -2597,8 +2833,11 @@
       <c r="H78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>11.57</v>
       </c>
@@ -2623,8 +2862,11 @@
       <c r="H79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>11.82</v>
       </c>
@@ -2649,8 +2891,11 @@
       <c r="H80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>11.66</v>
       </c>
@@ -2673,6 +2918,9 @@
         <v>1</v>
       </c>
       <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81">
         <v>0</v>
       </c>
     </row>
@@ -2683,15 +2931,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E846AE-E1CD-4571-B784-0E12F820FEBF}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" customWidth="1"/>
     <col min="2" max="2" width="71" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2765,6 +3013,14 @@
       </c>
       <c r="B9" s="2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>